<commit_message>
update S&P affirmation rating on July 30, 2024
</commit_message>
<xml_diff>
--- a/rating_tidy.xlsx
+++ b/rating_tidy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1731" yWindow="977" windowWidth="20734" windowHeight="11040" activeTab="3"/>
+    <workbookView xWindow="4073" yWindow="2360" windowWidth="20740" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="tidy_data" sheetId="6" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="234">
   <si>
     <t>Standard &amp; Poor's</t>
   </si>
@@ -718,6 +718,12 @@
   </si>
   <si>
     <t>Score</t>
+  </si>
+  <si>
+    <t>July 30, 2024</t>
+  </si>
+  <si>
+    <t>March 22, 2024</t>
   </si>
 </sst>
 </file>
@@ -825,7 +831,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -876,9 +882,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1159,22 +1169,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J137"/>
+  <dimension ref="A2:J139"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="B26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.7"/>
   <cols>
     <col min="1" max="1" width="18" style="26" customWidth="1"/>
     <col min="2" max="2" width="26" style="26" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" style="26" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" style="26" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" style="26" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="26" customWidth="1"/>
-    <col min="7" max="7" width="42.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="26"/>
+    <col min="3" max="3" width="25.88671875" style="26" customWidth="1"/>
+    <col min="4" max="4" width="29.109375" style="26" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" style="26" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" style="26" customWidth="1"/>
+    <col min="7" max="7" width="42.44140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="26"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
@@ -1266,7 +1276,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="40">
-        <f t="shared" ref="A7:A77" si="0">DATEVALUE(B7)</f>
+        <f t="shared" ref="A7:A78" si="0">DATEVALUE(B7)</f>
         <v>35804</v>
       </c>
       <c r="B7" s="31" t="s">
@@ -1503,16 +1513,16 @@
         <f t="shared" si="0"/>
         <v>37369</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="30" t="s">
+      <c r="C20" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="E20" s="38" t="s">
         <v>181</v>
       </c>
     </row>
@@ -1521,16 +1531,16 @@
         <f t="shared" si="0"/>
         <v>37504</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" s="30" t="s">
+      <c r="C21" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="30" t="s">
+      <c r="E21" s="38" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1539,16 +1549,16 @@
         <f t="shared" si="0"/>
         <v>37753</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="30" t="s">
+      <c r="C22" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="30" t="s">
+      <c r="E22" s="38" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1557,16 +1567,16 @@
         <f t="shared" si="0"/>
         <v>37902</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="30" t="s">
+      <c r="C23" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E23" s="38" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1575,16 +1585,16 @@
         <f t="shared" si="0"/>
         <v>38118</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="39" t="s">
         <v>186</v>
       </c>
-      <c r="C24" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="30" t="s">
+      <c r="C24" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="30" t="s">
+      <c r="E24" s="38" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1593,16 +1603,16 @@
         <f t="shared" si="0"/>
         <v>38343</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" s="30" t="s">
+      <c r="C25" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="30" t="s">
+      <c r="E25" s="38" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1611,16 +1621,16 @@
         <f t="shared" si="0"/>
         <v>38596</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="39" t="s">
         <v>187</v>
       </c>
-      <c r="C26" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="30" t="s">
+      <c r="C26" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="E26" s="38" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1629,16 +1639,16 @@
         <f t="shared" si="0"/>
         <v>38757</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="39" t="s">
         <v>188</v>
       </c>
-      <c r="C27" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D27" s="30" t="s">
+      <c r="C27" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="30" t="s">
+      <c r="E27" s="38" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1647,16 +1657,16 @@
         <f t="shared" si="0"/>
         <v>38924</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28" s="30" t="s">
+      <c r="C28" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="30" t="s">
+      <c r="E28" s="38" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1665,16 +1675,16 @@
         <f t="shared" si="0"/>
         <v>39759</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="35" t="s">
+      <c r="C29" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="35" t="s">
+      <c r="E29" s="38" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1683,16 +1693,16 @@
         <f t="shared" si="0"/>
         <v>40109</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" s="30" t="s">
+      <c r="C30" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="30" t="s">
+      <c r="E30" s="38" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1701,16 +1711,16 @@
         <f t="shared" si="0"/>
         <v>40249</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D31" s="30" t="s">
+      <c r="C31" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="38" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1719,16 +1729,16 @@
         <f t="shared" si="0"/>
         <v>40641</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="30" t="s">
+      <c r="C32" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="30" t="s">
+      <c r="E32" s="38" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1737,16 +1747,16 @@
         <f t="shared" si="0"/>
         <v>41022</v>
       </c>
-      <c r="B33" s="33" t="s">
+      <c r="B33" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="D33" s="35" t="s">
+      <c r="C33" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="35" t="s">
+      <c r="E33" s="38" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1755,16 +1765,16 @@
         <f t="shared" si="0"/>
         <v>41406</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34" s="30" t="s">
+      <c r="C34" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="30" t="s">
+      <c r="E34" s="38" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1773,16 +1783,16 @@
         <f t="shared" si="0"/>
         <v>41757</v>
       </c>
-      <c r="B35" s="33" t="s">
+      <c r="B35" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="D35" s="35" t="s">
+      <c r="C35" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="35" t="s">
+      <c r="E35" s="38" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1791,16 +1801,16 @@
         <f t="shared" si="0"/>
         <v>42145</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D36" s="30" t="s">
+      <c r="C36" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="E36" s="30" t="s">
+      <c r="E36" s="38" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1809,16 +1819,16 @@
         <f t="shared" si="0"/>
         <v>42522</v>
       </c>
-      <c r="B37" s="33" t="s">
+      <c r="B37" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="D37" s="35" t="s">
+      <c r="C37" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="35" t="s">
+      <c r="E37" s="38" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1827,16 +1837,16 @@
         <f t="shared" si="0"/>
         <v>42874</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" s="30" t="s">
+      <c r="C38" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="E38" s="30" t="s">
+      <c r="E38" s="38" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1845,16 +1855,16 @@
         <f t="shared" si="0"/>
         <v>43251</v>
       </c>
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" s="35" t="s">
+      <c r="C39" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="E39" s="35" t="s">
+      <c r="E39" s="38" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1863,16 +1873,16 @@
         <f t="shared" si="0"/>
         <v>43616</v>
       </c>
-      <c r="B40" s="31" t="s">
+      <c r="B40" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40" s="30" t="s">
+      <c r="C40" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="E40" s="30" t="s">
+      <c r="E40" s="38" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1881,16 +1891,16 @@
         <f t="shared" si="0"/>
         <v>43938</v>
       </c>
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D41" s="30" t="s">
+      <c r="C41" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="E41" s="30" t="s">
+      <c r="E41" s="38" t="s">
         <v>179</v>
       </c>
     </row>
@@ -1899,16 +1909,16 @@
         <f t="shared" si="0"/>
         <v>44308</v>
       </c>
-      <c r="B42" s="33" t="s">
+      <c r="B42" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="C42" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" s="35" t="s">
+      <c r="C42" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="E42" s="35" t="s">
+      <c r="E42" s="38" t="s">
         <v>179</v>
       </c>
     </row>
@@ -1917,16 +1927,16 @@
         <f t="shared" si="0"/>
         <v>44678</v>
       </c>
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="C43" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D43" s="30" t="s">
+      <c r="C43" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="E43" s="30" t="s">
+      <c r="E43" s="38" t="s">
         <v>178</v>
       </c>
       <c r="I43" s="27"/>
@@ -1937,82 +1947,82 @@
         <f t="shared" si="0"/>
         <v>45111</v>
       </c>
-      <c r="B44" s="33" t="s">
+      <c r="B44" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="C44" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D44" s="35" t="s">
+      <c r="C44" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="E44" s="30" t="s">
+      <c r="E44" s="38" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="40">
         <f t="shared" si="0"/>
-        <v>34407</v>
-      </c>
-      <c r="B45" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="C45" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D45" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E45" s="30"/>
+        <v>45503</v>
+      </c>
+      <c r="B45" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="35" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="40">
         <f t="shared" si="0"/>
-        <v>35785</v>
-      </c>
-      <c r="B46" s="37" t="s">
-        <v>61</v>
+        <v>34407</v>
+      </c>
+      <c r="B46" s="31" t="s">
+        <v>56</v>
       </c>
       <c r="C46" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D46" s="30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="40">
         <f t="shared" si="0"/>
-        <v>35804</v>
-      </c>
-      <c r="B47" s="31" t="s">
-        <v>28</v>
+        <v>35785</v>
+      </c>
+      <c r="B47" s="37" t="s">
+        <v>61</v>
       </c>
       <c r="C47" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D47" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="E47" s="30" t="s">
-        <v>178</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="E47" s="30"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="40">
         <f t="shared" si="0"/>
-        <v>35874</v>
+        <v>35804</v>
       </c>
       <c r="B48" s="31" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="C48" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D48" s="30" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="E48" s="30" t="s">
         <v>178</v>
@@ -2021,10 +2031,10 @@
     <row r="49" spans="1:5">
       <c r="A49" s="40">
         <f t="shared" si="0"/>
-        <v>37370</v>
+        <v>35874</v>
       </c>
       <c r="B49" s="31" t="s">
-        <v>191</v>
+        <v>62</v>
       </c>
       <c r="C49" s="30" t="s">
         <v>1</v>
@@ -2033,16 +2043,16 @@
         <v>76</v>
       </c>
       <c r="E49" s="30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="40">
         <f t="shared" si="0"/>
-        <v>37797</v>
+        <v>37370</v>
       </c>
       <c r="B50" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C50" s="30" t="s">
         <v>1</v>
@@ -2051,34 +2061,34 @@
         <v>76</v>
       </c>
       <c r="E50" s="30" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="40">
         <f t="shared" si="0"/>
-        <v>37893</v>
+        <v>37797</v>
       </c>
       <c r="B51" s="31" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C51" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="E51" s="30" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="40">
         <f t="shared" si="0"/>
-        <v>38401</v>
+        <v>37893</v>
       </c>
       <c r="B52" s="31" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C52" s="30" t="s">
         <v>1</v>
@@ -2087,16 +2097,16 @@
         <v>60</v>
       </c>
       <c r="E52" s="30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="40">
         <f t="shared" si="0"/>
-        <v>38774</v>
+        <v>38401</v>
       </c>
       <c r="B53" s="31" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C53" s="30" t="s">
         <v>1</v>
@@ -2105,34 +2115,34 @@
         <v>60</v>
       </c>
       <c r="E53" s="30" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="40">
         <f t="shared" si="0"/>
-        <v>38855</v>
+        <v>38774</v>
       </c>
       <c r="B54" s="31" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C54" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D54" s="30" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E54" s="30" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="40">
         <f t="shared" si="0"/>
-        <v>39118</v>
+        <v>38855</v>
       </c>
       <c r="B55" s="31" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C55" s="30" t="s">
         <v>1</v>
@@ -2141,16 +2151,16 @@
         <v>77</v>
       </c>
       <c r="E55" s="30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="40">
         <f t="shared" si="0"/>
-        <v>39295</v>
+        <v>39118</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C56" s="30" t="s">
         <v>1</v>
@@ -2159,34 +2169,34 @@
         <v>77</v>
       </c>
       <c r="E56" s="30" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="40">
         <f t="shared" si="0"/>
-        <v>39373</v>
+        <v>39295</v>
       </c>
       <c r="B57" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C57" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D57" s="30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E57" s="30" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="40">
         <f t="shared" si="0"/>
-        <v>39805</v>
+        <v>39373</v>
       </c>
       <c r="B58" s="31" t="s">
-        <v>66</v>
+        <v>200</v>
       </c>
       <c r="C58" s="30" t="s">
         <v>1</v>
@@ -2201,10 +2211,10 @@
     <row r="59" spans="1:5">
       <c r="A59" s="40">
         <f t="shared" si="0"/>
-        <v>39975</v>
+        <v>39805</v>
       </c>
       <c r="B59" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C59" s="30" t="s">
         <v>1</v>
@@ -2213,34 +2223,34 @@
         <v>78</v>
       </c>
       <c r="E59" s="30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="40">
         <f t="shared" si="0"/>
-        <v>40072</v>
+        <v>39975</v>
       </c>
       <c r="B60" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C60" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D60" s="30" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="E60" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="40">
         <f t="shared" si="0"/>
-        <v>40350</v>
+        <v>40072</v>
       </c>
       <c r="B61" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C61" s="30" t="s">
         <v>1</v>
@@ -2249,16 +2259,16 @@
         <v>59</v>
       </c>
       <c r="E61" s="30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="40">
         <f t="shared" si="0"/>
-        <v>40524</v>
+        <v>40350</v>
       </c>
       <c r="B62" s="31" t="s">
-        <v>201</v>
+        <v>69</v>
       </c>
       <c r="C62" s="30" t="s">
         <v>1</v>
@@ -2267,40 +2277,40 @@
         <v>59</v>
       </c>
       <c r="E62" s="30" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="40">
         <f t="shared" si="0"/>
-        <v>40560</v>
+        <v>40524</v>
       </c>
       <c r="B63" s="31" t="s">
-        <v>70</v>
+        <v>201</v>
       </c>
       <c r="C63" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D63" s="30" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E63" s="30" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="40">
         <f t="shared" si="0"/>
-        <v>40926</v>
+        <v>40560</v>
       </c>
       <c r="B64" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C64" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D64" s="30" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E64" s="30" t="s">
         <v>178</v>
@@ -2309,10 +2319,10 @@
     <row r="65" spans="1:5">
       <c r="A65" s="40">
         <f t="shared" si="0"/>
-        <v>42397</v>
+        <v>40926</v>
       </c>
       <c r="B65" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C65" s="30" t="s">
         <v>1</v>
@@ -2327,10 +2337,10 @@
     <row r="66" spans="1:5">
       <c r="A66" s="40">
         <f t="shared" si="0"/>
-        <v>42774</v>
+        <v>42397</v>
       </c>
       <c r="B66" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C66" s="30" t="s">
         <v>1</v>
@@ -2339,34 +2349,34 @@
         <v>57</v>
       </c>
       <c r="E66" s="30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="40">
         <f t="shared" si="0"/>
-        <v>43203</v>
+        <v>42774</v>
       </c>
       <c r="B67" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C67" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D67" s="30" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="E67" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="40">
         <f t="shared" si="0"/>
-        <v>43871</v>
+        <v>43203</v>
       </c>
       <c r="B68" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C68" s="30" t="s">
         <v>1</v>
@@ -2381,10 +2391,10 @@
     <row r="69" spans="1:5">
       <c r="A69" s="40">
         <f t="shared" si="0"/>
-        <v>44222</v>
+        <v>43871</v>
       </c>
       <c r="B69" s="31" t="s">
-        <v>146</v>
+        <v>75</v>
       </c>
       <c r="C69" s="30" t="s">
         <v>1</v>
@@ -2399,10 +2409,10 @@
     <row r="70" spans="1:5">
       <c r="A70" s="40">
         <f t="shared" si="0"/>
-        <v>44602</v>
+        <v>44222</v>
       </c>
       <c r="B70" s="31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C70" s="30" t="s">
         <v>1</v>
@@ -2417,15 +2427,15 @@
     <row r="71" spans="1:5">
       <c r="A71" s="40">
         <f t="shared" si="0"/>
-        <v>45398</v>
-      </c>
-      <c r="B71" s="35" t="s">
-        <v>171</v>
+        <v>44602</v>
+      </c>
+      <c r="B71" s="31" t="s">
+        <v>147</v>
       </c>
       <c r="C71" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D71" s="35" t="s">
+      <c r="D71" s="30" t="s">
         <v>84</v>
       </c>
       <c r="E71" s="30" t="s">
@@ -2435,170 +2445,172 @@
     <row r="72" spans="1:5">
       <c r="A72" s="40">
         <f t="shared" si="0"/>
-        <v>35582</v>
-      </c>
-      <c r="B72" s="31" t="s">
-        <v>86</v>
+        <v>45398</v>
+      </c>
+      <c r="B72" s="35" t="s">
+        <v>171</v>
       </c>
       <c r="C72" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D72" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E72" s="30"/>
+        <v>1</v>
+      </c>
+      <c r="D72" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="E72" s="30" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="40">
         <f t="shared" si="0"/>
-        <v>35787</v>
+        <v>35582</v>
       </c>
       <c r="B73" s="31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C73" s="30" t="s">
         <v>2</v>
       </c>
       <c r="D73" s="30" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E73" s="30"/>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="40">
         <f t="shared" si="0"/>
-        <v>35803</v>
+        <v>35787</v>
       </c>
       <c r="B74" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C74" s="30" t="s">
         <v>2</v>
       </c>
       <c r="D74" s="30" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E74" s="30"/>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="40">
         <f t="shared" si="0"/>
-        <v>35816</v>
+        <v>35803</v>
       </c>
       <c r="B75" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C75" s="30" t="s">
         <v>2</v>
       </c>
       <c r="D75" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E75" s="30"/>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="40">
         <f t="shared" si="0"/>
-        <v>35870</v>
+        <v>35816</v>
       </c>
       <c r="B76" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C76" s="30" t="s">
         <v>2</v>
       </c>
       <c r="D76" s="30" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E76" s="30"/>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="40">
         <f t="shared" si="0"/>
-        <v>37469</v>
+        <v>35870</v>
       </c>
       <c r="B77" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C77" s="30" t="s">
         <v>2</v>
       </c>
       <c r="D77" s="30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E77" s="30"/>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="40">
-        <f t="shared" ref="A78:A137" si="1">DATEVALUE(B78)</f>
-        <v>37945</v>
+        <f t="shared" si="0"/>
+        <v>37469</v>
       </c>
       <c r="B78" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C78" s="30" t="s">
         <v>2</v>
       </c>
       <c r="D78" s="30" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E78" s="30"/>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="40">
-        <f t="shared" si="1"/>
-        <v>38379</v>
+        <f t="shared" ref="A79:A139" si="1">DATEVALUE(B79)</f>
+        <v>37945</v>
       </c>
       <c r="B79" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C79" s="30" t="s">
         <v>2</v>
       </c>
       <c r="D79" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E79" s="30"/>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="40">
         <f t="shared" si="1"/>
-        <v>39492</v>
+        <v>38379</v>
       </c>
       <c r="B80" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C80" s="30" t="s">
         <v>2</v>
       </c>
       <c r="D80" s="30" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E80" s="30"/>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="40">
         <f t="shared" si="1"/>
-        <v>40892</v>
+        <v>39492</v>
       </c>
       <c r="B81" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C81" s="30" t="s">
         <v>2</v>
       </c>
       <c r="D81" s="30" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E81" s="30"/>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="40">
         <f t="shared" si="1"/>
-        <v>41235</v>
+        <v>40892</v>
       </c>
       <c r="B82" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C82" s="30" t="s">
         <v>2</v>
@@ -2611,10 +2623,10 @@
     <row r="83" spans="1:5">
       <c r="A83" s="40">
         <f t="shared" si="1"/>
-        <v>41593</v>
+        <v>41235</v>
       </c>
       <c r="B83" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C83" s="30" t="s">
         <v>2</v>
@@ -2627,10 +2639,10 @@
     <row r="84" spans="1:5">
       <c r="A84" s="40">
         <f t="shared" si="1"/>
-        <v>41956</v>
+        <v>41593</v>
       </c>
       <c r="B84" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C84" s="30" t="s">
         <v>2</v>
@@ -2643,10 +2655,10 @@
     <row r="85" spans="1:5">
       <c r="A85" s="40">
         <f t="shared" si="1"/>
-        <v>42314</v>
+        <v>41956</v>
       </c>
       <c r="B85" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C85" s="30" t="s">
         <v>2</v>
@@ -2659,10 +2671,10 @@
     <row r="86" spans="1:5">
       <c r="A86" s="40">
         <f t="shared" si="1"/>
-        <v>42513</v>
+        <v>42314</v>
       </c>
       <c r="B86" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C86" s="30" t="s">
         <v>2</v>
@@ -2670,17 +2682,15 @@
       <c r="D86" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E86" s="30" t="s">
-        <v>178</v>
-      </c>
+      <c r="E86" s="30"/>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="40">
         <f t="shared" si="1"/>
-        <v>42725</v>
+        <v>42513</v>
       </c>
       <c r="B87" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C87" s="30" t="s">
         <v>2</v>
@@ -2689,16 +2699,16 @@
         <v>6</v>
       </c>
       <c r="E87" s="30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="40">
         <f t="shared" si="1"/>
-        <v>42935</v>
+        <v>42725</v>
       </c>
       <c r="B88" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C88" s="30" t="s">
         <v>2</v>
@@ -2706,31 +2716,33 @@
       <c r="D88" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E88" s="30"/>
+      <c r="E88" s="30" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="40">
         <f t="shared" si="1"/>
-        <v>43454</v>
+        <v>42935</v>
       </c>
       <c r="B89" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C89" s="30" t="s">
         <v>2</v>
       </c>
       <c r="D89" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E89" s="30"/>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="40">
         <f t="shared" si="1"/>
-        <v>43538</v>
+        <v>43454</v>
       </c>
       <c r="B90" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C90" s="30" t="s">
         <v>2</v>
@@ -2743,10 +2755,10 @@
     <row r="91" spans="1:5">
       <c r="A91" s="40">
         <f t="shared" si="1"/>
-        <v>43854</v>
+        <v>43538</v>
       </c>
       <c r="B91" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C91" s="30" t="s">
         <v>2</v>
@@ -2759,15 +2771,15 @@
     <row r="92" spans="1:5">
       <c r="A92" s="40">
         <f t="shared" si="1"/>
-        <v>44277</v>
+        <v>43854</v>
       </c>
       <c r="B92" s="31" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
       <c r="C92" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D92" s="38" t="s">
+      <c r="D92" s="30" t="s">
         <v>7</v>
       </c>
       <c r="E92" s="30"/>
@@ -2775,10 +2787,10 @@
     <row r="93" spans="1:5">
       <c r="A93" s="40">
         <f t="shared" si="1"/>
-        <v>44522</v>
+        <v>44277</v>
       </c>
       <c r="B93" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C93" s="30" t="s">
         <v>2</v>
@@ -2791,10 +2803,10 @@
     <row r="94" spans="1:5">
       <c r="A94" s="40">
         <f t="shared" si="1"/>
-        <v>44740</v>
+        <v>44522</v>
       </c>
       <c r="B94" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C94" s="30" t="s">
         <v>2</v>
@@ -2807,15 +2819,15 @@
     <row r="95" spans="1:5">
       <c r="A95" s="40">
         <f t="shared" si="1"/>
-        <v>44909</v>
+        <v>44740</v>
       </c>
       <c r="B95" s="31" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C95" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D95" s="30" t="s">
+      <c r="D95" s="38" t="s">
         <v>7</v>
       </c>
       <c r="E95" s="30"/>
@@ -2823,15 +2835,15 @@
     <row r="96" spans="1:5">
       <c r="A96" s="40">
         <f t="shared" si="1"/>
-        <v>45170</v>
-      </c>
-      <c r="B96" s="38" t="s">
-        <v>170</v>
+        <v>44909</v>
+      </c>
+      <c r="B96" s="31" t="s">
+        <v>156</v>
       </c>
       <c r="C96" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D96" s="38" t="s">
+      <c r="D96" s="30" t="s">
         <v>7</v>
       </c>
       <c r="E96" s="30"/>
@@ -2839,92 +2851,92 @@
     <row r="97" spans="1:5">
       <c r="A97" s="40">
         <f t="shared" si="1"/>
-        <v>45366</v>
-      </c>
-      <c r="B97" s="35" t="s">
-        <v>172</v>
+        <v>45170</v>
+      </c>
+      <c r="B97" s="38" t="s">
+        <v>170</v>
       </c>
       <c r="C97" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D97" s="35" t="s">
+      <c r="D97" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="E97" s="30" t="s">
-        <v>178</v>
-      </c>
+      <c r="E97" s="30"/>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="40">
         <f t="shared" si="1"/>
-        <v>35929</v>
-      </c>
-      <c r="B98" s="31" t="s">
-        <v>108</v>
+        <v>45366</v>
+      </c>
+      <c r="B98" s="35" t="s">
+        <v>172</v>
       </c>
       <c r="C98" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="D98" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="E98" s="30"/>
+        <v>2</v>
+      </c>
+      <c r="D98" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E98" s="30" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="40">
         <f t="shared" si="1"/>
-        <v>36431</v>
+        <v>35929</v>
       </c>
       <c r="B99" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C99" s="30" t="s">
         <v>3</v>
       </c>
       <c r="D99" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E99" s="30"/>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="40">
         <f t="shared" si="1"/>
-        <v>38146</v>
+        <v>36431</v>
       </c>
       <c r="B100" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C100" s="30" t="s">
         <v>3</v>
       </c>
       <c r="D100" s="30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E100" s="30"/>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="40">
         <f t="shared" si="1"/>
-        <v>38555</v>
+        <v>38146</v>
       </c>
       <c r="B101" s="31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C101" s="30" t="s">
         <v>3</v>
       </c>
       <c r="D101" s="30" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E101" s="30"/>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="40">
         <f t="shared" si="1"/>
-        <v>39002</v>
+        <v>38555</v>
       </c>
       <c r="B102" s="31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C102" s="30" t="s">
         <v>3</v>
@@ -2937,26 +2949,26 @@
     <row r="103" spans="1:5">
       <c r="A103" s="40">
         <f t="shared" si="1"/>
-        <v>39386</v>
+        <v>39002</v>
       </c>
       <c r="B103" s="31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C103" s="30" t="s">
         <v>3</v>
       </c>
       <c r="D103" s="30" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E103" s="30"/>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="40">
         <f t="shared" si="1"/>
-        <v>39827</v>
+        <v>39386</v>
       </c>
       <c r="B104" s="31" t="s">
-        <v>190</v>
+        <v>113</v>
       </c>
       <c r="C104" s="30" t="s">
         <v>3</v>
@@ -2969,10 +2981,10 @@
     <row r="105" spans="1:5">
       <c r="A105" s="40">
         <f t="shared" si="1"/>
-        <v>40093</v>
+        <v>39827</v>
       </c>
       <c r="B105" s="31" t="s">
-        <v>115</v>
+        <v>190</v>
       </c>
       <c r="C105" s="30" t="s">
         <v>3</v>
@@ -2980,17 +2992,15 @@
       <c r="D105" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E105" s="30" t="s">
-        <v>178</v>
-      </c>
+      <c r="E105" s="30"/>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="40">
         <f t="shared" si="1"/>
-        <v>40465</v>
+        <v>40093</v>
       </c>
       <c r="B106" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C106" s="30" t="s">
         <v>3</v>
@@ -2999,16 +3009,16 @@
         <v>8</v>
       </c>
       <c r="E106" s="30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="40">
         <f t="shared" si="1"/>
-        <v>40861</v>
+        <v>40465</v>
       </c>
       <c r="B107" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C107" s="30" t="s">
         <v>3</v>
@@ -3016,31 +3026,33 @@
       <c r="D107" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E107" s="30"/>
+      <c r="E107" s="30" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="40">
         <f t="shared" si="1"/>
-        <v>41200</v>
+        <v>40861</v>
       </c>
       <c r="B108" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C108" s="30" t="s">
         <v>3</v>
       </c>
       <c r="D108" s="30" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E108" s="30"/>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="40">
         <f t="shared" si="1"/>
-        <v>41558</v>
+        <v>41200</v>
       </c>
       <c r="B109" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C109" s="30" t="s">
         <v>3</v>
@@ -3053,10 +3065,10 @@
     <row r="110" spans="1:5">
       <c r="A110" s="40">
         <f t="shared" si="1"/>
-        <v>42081</v>
+        <v>41558</v>
       </c>
       <c r="B110" s="31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C110" s="30" t="s">
         <v>3</v>
@@ -3069,10 +3081,10 @@
     <row r="111" spans="1:5">
       <c r="A111" s="40">
         <f t="shared" si="1"/>
-        <v>42464</v>
+        <v>42081</v>
       </c>
       <c r="B111" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C111" s="30" t="s">
         <v>3</v>
@@ -3080,17 +3092,15 @@
       <c r="D111" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E111" s="30" t="s">
-        <v>178</v>
-      </c>
+      <c r="E111" s="30"/>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="40">
         <f t="shared" si="1"/>
-        <v>42830</v>
+        <v>42464</v>
       </c>
       <c r="B112" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C112" s="30" t="s">
         <v>3</v>
@@ -3099,32 +3109,34 @@
         <v>6</v>
       </c>
       <c r="E112" s="30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="40">
         <f t="shared" si="1"/>
-        <v>43166</v>
+        <v>42830</v>
       </c>
       <c r="B113" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C113" s="30" t="s">
         <v>3</v>
       </c>
       <c r="D113" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="E113" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="E113" s="30" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="40">
         <f t="shared" si="1"/>
-        <v>43581</v>
+        <v>43166</v>
       </c>
       <c r="B114" s="31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C114" s="30" t="s">
         <v>3</v>
@@ -3137,26 +3149,26 @@
     <row r="115" spans="1:5">
       <c r="A115" s="40">
         <f t="shared" si="1"/>
-        <v>43907</v>
-      </c>
-      <c r="B115" s="39" t="s">
-        <v>126</v>
+        <v>43581</v>
+      </c>
+      <c r="B115" s="31" t="s">
+        <v>124</v>
       </c>
       <c r="C115" s="30" t="s">
         <v>3</v>
       </c>
       <c r="D115" s="30" t="s">
-        <v>125</v>
+        <v>7</v>
       </c>
       <c r="E115" s="30"/>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="40">
         <f t="shared" si="1"/>
-        <v>44308</v>
-      </c>
-      <c r="B116" s="31" t="s">
-        <v>152</v>
+        <v>43907</v>
+      </c>
+      <c r="B116" s="39" t="s">
+        <v>126</v>
       </c>
       <c r="C116" s="30" t="s">
         <v>3</v>
@@ -3169,10 +3181,10 @@
     <row r="117" spans="1:5">
       <c r="A117" s="40">
         <f t="shared" si="1"/>
-        <v>44746</v>
-      </c>
-      <c r="B117" s="39" t="s">
-        <v>161</v>
+        <v>44308</v>
+      </c>
+      <c r="B117" s="31" t="s">
+        <v>152</v>
       </c>
       <c r="C117" s="30" t="s">
         <v>3</v>
@@ -3180,17 +3192,15 @@
       <c r="D117" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="E117" s="30" t="s">
-        <v>177</v>
-      </c>
+      <c r="E117" s="30"/>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="40">
         <f t="shared" si="1"/>
-        <v>45132</v>
-      </c>
-      <c r="B118" s="33" t="s">
-        <v>165</v>
+        <v>44746</v>
+      </c>
+      <c r="B118" s="39" t="s">
+        <v>161</v>
       </c>
       <c r="C118" s="30" t="s">
         <v>3</v>
@@ -3205,74 +3215,76 @@
     <row r="119" spans="1:5">
       <c r="A119" s="40">
         <f t="shared" si="1"/>
-        <v>37554</v>
-      </c>
-      <c r="B119" s="31" t="s">
-        <v>127</v>
+        <v>45132</v>
+      </c>
+      <c r="B119" s="33" t="s">
+        <v>165</v>
       </c>
       <c r="C119" s="30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D119" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="E119" s="30"/>
+        <v>125</v>
+      </c>
+      <c r="E119" s="30" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="40">
         <f t="shared" si="1"/>
-        <v>38133</v>
+        <v>37554</v>
       </c>
       <c r="B120" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C120" s="30" t="s">
         <v>4</v>
       </c>
       <c r="D120" s="30" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E120" s="30"/>
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="40">
         <f t="shared" si="1"/>
-        <v>38981</v>
+        <v>38133</v>
       </c>
       <c r="B121" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C121" s="30" t="s">
         <v>4</v>
       </c>
       <c r="D121" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E121" s="30"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="40">
         <f t="shared" si="1"/>
-        <v>39332</v>
+        <v>38981</v>
       </c>
       <c r="B122" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C122" s="30" t="s">
         <v>4</v>
       </c>
       <c r="D122" s="30" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E122" s="30"/>
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="40">
         <f t="shared" si="1"/>
-        <v>39716</v>
+        <v>39332</v>
       </c>
       <c r="B123" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C123" s="30" t="s">
         <v>4</v>
@@ -3285,10 +3297,10 @@
     <row r="124" spans="1:5">
       <c r="A124" s="40">
         <f t="shared" si="1"/>
-        <v>39849</v>
+        <v>39716</v>
       </c>
       <c r="B124" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C124" s="30" t="s">
         <v>4</v>
@@ -3301,42 +3313,42 @@
     <row r="125" spans="1:5">
       <c r="A125" s="40">
         <f t="shared" si="1"/>
-        <v>40001</v>
+        <v>39849</v>
       </c>
       <c r="B125" s="31" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C125" s="30" t="s">
         <v>4</v>
       </c>
       <c r="D125" s="30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E125" s="30"/>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="40">
         <f t="shared" si="1"/>
-        <v>40372</v>
+        <v>40001</v>
       </c>
       <c r="B126" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C126" s="30" t="s">
         <v>4</v>
       </c>
       <c r="D126" s="30" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E126" s="30"/>
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="40">
         <f t="shared" si="1"/>
-        <v>40779</v>
+        <v>40372</v>
       </c>
       <c r="B127" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C127" s="30" t="s">
         <v>4</v>
@@ -3349,10 +3361,10 @@
     <row r="128" spans="1:5">
       <c r="A128" s="40">
         <f t="shared" si="1"/>
-        <v>41226</v>
+        <v>40779</v>
       </c>
       <c r="B128" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C128" s="30" t="s">
         <v>4</v>
@@ -3365,10 +3377,10 @@
     <row r="129" spans="1:5">
       <c r="A129" s="40">
         <f t="shared" si="1"/>
-        <v>41477</v>
+        <v>41226</v>
       </c>
       <c r="B129" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C129" s="30" t="s">
         <v>4</v>
@@ -3381,10 +3393,10 @@
     <row r="130" spans="1:5">
       <c r="A130" s="40">
         <f t="shared" si="1"/>
-        <v>41934</v>
+        <v>41477</v>
       </c>
       <c r="B130" s="31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C130" s="30" t="s">
         <v>4</v>
@@ -3397,10 +3409,10 @@
     <row r="131" spans="1:5">
       <c r="A131" s="40">
         <f t="shared" si="1"/>
-        <v>42401</v>
+        <v>41934</v>
       </c>
       <c r="B131" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C131" s="30" t="s">
         <v>4</v>
@@ -3408,17 +3420,15 @@
       <c r="D131" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E131" s="30" t="s">
-        <v>178</v>
-      </c>
+      <c r="E131" s="30"/>
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="40">
         <f t="shared" si="1"/>
-        <v>42801</v>
+        <v>42401</v>
       </c>
       <c r="B132" s="31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C132" s="30" t="s">
         <v>4</v>
@@ -3427,34 +3437,34 @@
         <v>6</v>
       </c>
       <c r="E132" s="30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="40">
         <f t="shared" si="1"/>
-        <v>43139</v>
+        <v>42801</v>
       </c>
       <c r="B133" s="31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C133" s="30" t="s">
         <v>4</v>
       </c>
       <c r="D133" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E133" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="40">
         <f t="shared" si="1"/>
-        <v>43581</v>
+        <v>43139</v>
       </c>
       <c r="B134" s="31" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="C134" s="30" t="s">
         <v>4</v>
@@ -3463,37 +3473,39 @@
         <v>7</v>
       </c>
       <c r="E134" s="30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="40">
         <f t="shared" si="1"/>
-        <v>43861</v>
+        <v>43581</v>
       </c>
       <c r="B135" s="31" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="C135" s="30" t="s">
         <v>4</v>
       </c>
       <c r="D135" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="E135" s="30"/>
+        <v>7</v>
+      </c>
+      <c r="E135" s="30" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="40">
         <f t="shared" si="1"/>
-        <v>44187</v>
-      </c>
-      <c r="B136" s="39" t="s">
-        <v>162</v>
+        <v>43861</v>
+      </c>
+      <c r="B136" s="31" t="s">
+        <v>144</v>
       </c>
       <c r="C136" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D136" s="38" t="s">
+      <c r="D136" s="30" t="s">
         <v>125</v>
       </c>
       <c r="E136" s="30"/>
@@ -3501,18 +3513,54 @@
     <row r="137" spans="1:5">
       <c r="A137" s="40">
         <f t="shared" si="1"/>
-        <v>44764</v>
-      </c>
-      <c r="B137" s="35" t="s">
-        <v>163</v>
+        <v>44187</v>
+      </c>
+      <c r="B137" s="39" t="s">
+        <v>162</v>
       </c>
       <c r="C137" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D137" s="35" t="s">
+      <c r="D137" s="38" t="s">
         <v>125</v>
       </c>
       <c r="E137" s="30"/>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" s="45">
+        <f t="shared" si="1"/>
+        <v>44764</v>
+      </c>
+      <c r="B138" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="C138" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D138" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="E138" s="30" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" s="40">
+        <f t="shared" si="1"/>
+        <v>45373</v>
+      </c>
+      <c r="B139" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="C139" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D139" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="E139" s="26" t="s">
+        <v>178</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3524,44 +3572,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K51"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="74" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="74" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="13.7"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" customWidth="1"/>
-    <col min="10" max="10" width="26.85546875" customWidth="1"/>
+    <col min="8" max="8" width="23.109375" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" customWidth="1"/>
+    <col min="10" max="10" width="26.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11">
-      <c r="B2" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44" t="s">
+      <c r="B2" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44" t="s">
+      <c r="E2" s="46"/>
+      <c r="F2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44" t="s">
+      <c r="G2" s="46"/>
+      <c r="H2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44" t="s">
+      <c r="I2" s="46"/>
+      <c r="J2" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="44"/>
+      <c r="K2" s="46"/>
     </row>
     <row r="3" spans="2:11">
       <c r="B3" s="3" t="s">
@@ -4164,10 +4212,10 @@
       <c r="I21" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="J21" s="9" t="s">
+      <c r="J21" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="K21" s="9" t="s">
+      <c r="K21" s="18" t="s">
         <v>160</v>
       </c>
     </row>
@@ -4194,6 +4242,12 @@
         <v>161</v>
       </c>
       <c r="I22" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="K22" s="9" t="s">
         <v>160</v>
       </c>
     </row>
@@ -4416,10 +4470,10 @@
       <c r="K37" s="4"/>
     </row>
     <row r="38" spans="2:11">
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="17" t="s">
         <v>88</v>
       </c>
       <c r="D38" s="22"/>
@@ -4432,8 +4486,12 @@
       <c r="K38" s="22"/>
     </row>
     <row r="39" spans="2:11">
-      <c r="B39" s="8"/>
-      <c r="C39" s="9"/>
+      <c r="B39" s="44" t="s">
+        <v>232</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>88</v>
+      </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
@@ -4508,16 +4566,16 @@
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.7"/>
   <cols>
     <col min="1" max="1" width="18" style="26" customWidth="1"/>
     <col min="2" max="2" width="26" style="26" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" style="26" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="26" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" style="26" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="26" customWidth="1"/>
-    <col min="7" max="7" width="42.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="26"/>
+    <col min="3" max="3" width="25.88671875" style="26" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="26" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" style="26" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" style="26" customWidth="1"/>
+    <col min="7" max="7" width="42.44140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="26"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
@@ -6867,15 +6925,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="13.7"/>
   <cols>
-    <col min="1" max="1" width="36.140625" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="36.109375" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>